<commit_message>
Move _fore_DX.pkl and silver_fore.xlsx from artifacts to root directory
</commit_message>
<xml_diff>
--- a/silver_fore.xlsx
+++ b/silver_fore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,25 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">   SILVER_FOR</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>SILVER_FOR</t>
         </is>
@@ -458,9 +468,15 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>27.44466</v>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -470,9 +486,15 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
         <v>26.933548</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -482,9 +504,15 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
         <v>27.173124</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -494,9 +522,15 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
         <v>26.856646</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -506,17 +540,29 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
         <v>26.422922</v>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
         <v>30.93059290717292</v>
       </c>
     </row>
@@ -524,9 +570,15 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
         <v>30.6353459147918</v>
       </c>
     </row>
@@ -534,9 +586,15 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
         <v>30.30023174736436</v>
       </c>
     </row>
@@ -544,9 +602,15 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
         <v>29.53532024840348</v>
       </c>
     </row>
@@ -554,10 +618,146 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
         <v>29.15916464141611</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>31.76244298992617</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>32.23934168175691</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>32.5524573182023</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>32.38868114596181</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>32.10415671664822</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>28.81685345771996</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>28.51061683625062</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>27.67123246313037</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>27.34084839285276</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>26.94339908891732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>